<commit_message>
Fouten in database opgelost
</commit_message>
<xml_diff>
--- a/Actuele menu brandstofcafe.xlsx
+++ b/Actuele menu brandstofcafe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\OneDrive\Documenten\Repos\project-webdeployment-groep_11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3F5998-F648-49C7-947C-1FA6B3744366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB400B6-E564-4949-BE9D-02D2F7A674F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{98019DCA-B281-4028-AF9C-A7331D3D849D}"/>
   </bookViews>
@@ -910,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4535FE9C-C56C-4123-9AB4-19657575B388}">
   <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="79" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:K49"/>
+    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>